<commit_message>
Updated Azure DevOps import IP list
</commit_message>
<xml_diff>
--- a/extra/Azure DevOps IPs.xlsx
+++ b/extra/Azure DevOps IPs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD41ED7-418C-4526-8A29-E3B13076C3EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520C5A2A-4E78-4494-8D17-3FF4147460EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Service</t>
   </si>
@@ -58,15 +63,9 @@
     <t>Regional Identity Service - Australia East 1</t>
   </si>
   <si>
-    <t>13.70.121.123</t>
-  </si>
-  <si>
     <t>Regional Identity Service - Australia East 2</t>
   </si>
   <si>
-    <t>52.187.228.246</t>
-  </si>
-  <si>
     <t>Data Migration tool - Australia East 1</t>
   </si>
   <si>
@@ -161,6 +160,33 @@
   </si>
   <si>
     <t>40.82.221.14</t>
+  </si>
+  <si>
+    <t>Regional Identity Service - Australia East 3</t>
+  </si>
+  <si>
+    <t>Regional Identity Service - Australia East 4</t>
+  </si>
+  <si>
+    <t>Regional Identity Service - Australia East 5</t>
+  </si>
+  <si>
+    <t>Regional Identity Service - Australia East 6</t>
+  </si>
+  <si>
+    <t>20.37.194.0/24</t>
+  </si>
+  <si>
+    <t>Test Plans - Australia East 1</t>
+  </si>
+  <si>
+    <t>20.40.177.101</t>
+  </si>
+  <si>
+    <t>Analytics service - Australia East 1</t>
+  </si>
+  <si>
+    <t>20.40.179.159</t>
   </si>
 </sst>
 </file>
@@ -555,9 +581,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -600,7 +628,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D23" si="0">"@{
+        <f t="shared" ref="D3:D29" si="0">"@{
     serviceName = '" &amp; A3 &amp; "'; 
     IPs = '" &amp; B3 &amp; "';
 },"</f>
@@ -615,39 +643,99 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Regional Identity Service - Australia East 1'; 
-    IPs = '13.70.121.123';
+    IPs = '13.75.145.145';
 },</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Regional Identity Service - Australia East 2'; 
-    IPs = '52.187.228.246';
+    IPs = '40.82.217.103';
 },</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>@{
+    serviceName = 'Regional Identity Service - Australia East 3'; 
+    IPs = '20.188.213.113';
+},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>@{
+    serviceName = 'Regional Identity Service - Australia East 4'; 
+    IPs = '104.210.88.194';
+},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>@{
+    serviceName = 'Regional Identity Service - Australia East 5'; 
+    IPs = '40.81.62.114';
+},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>@{
+    serviceName = 'Regional Identity Service - Australia East 6'; 
+    IPs = '20.37.194.0/24';
+},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Data Migration tool - Australia East 1'; 
@@ -655,14 +743,14 @@
 },</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="str">
+    <row r="11" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Data Migration tool - Australia East 2'; 
@@ -670,14 +758,14 @@
 },</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="str">
+    <row r="12" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Data Migration tool - Australia East 3'; 
@@ -685,14 +773,14 @@
 },</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="str">
+    <row r="13" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure DevOps Services - Australia East 1'; 
@@ -700,14 +788,14 @@
 },</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="str">
+    <row r="14" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure DevOps Services - Australia East 2'; 
@@ -715,14 +803,14 @@
 },</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="str">
+    <row r="15" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure DevOps Services - Australia East 3'; 
@@ -730,14 +818,14 @@
 },</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="str">
+    <row r="16" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure DevOps Services - Australia East 4'; 
@@ -745,14 +833,14 @@
 },</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="str">
+    <row r="17" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure DevOps Services - Australia East 5'; 
@@ -760,14 +848,14 @@
 },</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="4" t="s">
+    <row r="18" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D14" t="str">
+      <c r="D18" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Releases service - Australia East 1'; 
@@ -775,14 +863,14 @@
 },</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="str">
+    <row r="19" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Releases service - Australia East 2'; 
@@ -790,14 +878,14 @@
 },</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="4" t="s">
+    <row r="20" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D16" t="str">
+      <c r="D20" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure Artifacts - Australia East 1'; 
@@ -805,14 +893,14 @@
 },</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="str">
+    <row r="21" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure Artifacts - Australia East 2'; 
@@ -820,14 +908,14 @@
 },</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="str">
+    <row r="22" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure Artifacts - Australia East 3'; 
@@ -835,14 +923,14 @@
 },</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="4" t="s">
+    <row r="23" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="str">
+      <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure Artifacts Feed - Australia East 1'; 
@@ -850,14 +938,14 @@
 },</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="str">
+    <row r="24" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure Artifacts Feed - Australia East 2'; 
@@ -865,14 +953,14 @@
 },</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" t="str">
+    <row r="25" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure Artifacts Blob - Australia East 1'; 
@@ -880,14 +968,14 @@
 },</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" t="str">
+    <row r="26" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure Artifacts Blob - Australia East 2'; 
@@ -895,18 +983,48 @@
 },</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" t="str">
+    <row r="27" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" t="str">
         <f t="shared" si="0"/>
         <v>@{
     serviceName = 'Azure Artifacts Blob - Australia East 3'; 
     IPs = '40.82.221.14';
+},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>@{
+    serviceName = 'Test Plans - Australia East 1'; 
+    IPs = '20.40.177.101';
+},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>@{
+    serviceName = 'Analytics service - Australia East 1'; 
+    IPs = '20.40.179.159';
 },</v>
       </c>
     </row>
@@ -914,4 +1032,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>